<commit_message>
update ESD excel file
</commit_message>
<xml_diff>
--- a/inst/concepts/ESD_concepts.xlsx
+++ b/inst/concepts/ESD_concepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ablack/darwin/PregnancyIdentifier/inst/concepts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38ECC311-D1B8-1047-8CF3-671EB558F052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC4066E-FC9F-ED4A-98C1-70588DDE7DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="21520" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7900" yWindow="2180" windowWidth="26540" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
   <si>
     <t>3011536</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Observation</t>
   </si>
   <si>
-    <t>observationConceptIds</t>
-  </si>
-  <si>
     <t>3026070</t>
   </si>
   <si>
@@ -56,18 +53,6 @@
   </si>
   <si>
     <t>gestAtBirthConceptIds</t>
-  </si>
-  <si>
-    <t>40758410</t>
-  </si>
-  <si>
-    <t>Number of fetuses</t>
-  </si>
-  <si>
-    <t>3002549</t>
-  </si>
-  <si>
-    <t>Number of fetuses by US</t>
   </si>
   <si>
     <t>43054890</t>
@@ -309,10 +294,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8206DE2B-3158-6F46-B03B-6A61C65F4D3B}" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0">
-  <autoFilter ref="A1:D34" xr:uid="{8206DE2B-3158-6F46-B03B-6A61C65F4D3B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D34">
-    <sortCondition ref="D1:D34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8206DE2B-3158-6F46-B03B-6A61C65F4D3B}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0">
+  <autoFilter ref="A1:D32" xr:uid="{8206DE2B-3158-6F46-B03B-6A61C65F4D3B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D32">
+    <sortCondition ref="D1:D32"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{393A83AA-A4F6-164F-9EA5-E290BDCF58FD}" name="esd_concept_id"/>
@@ -603,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -619,408 +604,408 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
       <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
         <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
         <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1034,63 +1019,35 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
         <v>6</v>
       </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>